<commit_message>
Aggiunta bozza del ppt, contenente il livello 1 quasi completo.
</commit_message>
<xml_diff>
--- a/L2/ManzoGray/FF 10% conf C/pivot.xlsx
+++ b/L2/ManzoGray/FF 10% conf C/pivot.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alessio\git\OMA-1516---Group-21\L2\ManzoGray\FF 10% conf C\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="124519"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId2"/>
+    <pivotCache cacheId="0" r:id="rId2"/>
   </pivotCaches>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -149,8 +144,18 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000%"/>
+  </numFmts>
+  <fonts count="2">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,19 +181,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Percentuale" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2244,7 +2252,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabella_pivot1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabella_pivot1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:E37" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
@@ -2471,7 +2479,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2506,7 +2514,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2683,21 +2691,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K4" sqref="K4:K36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
@@ -2706,7 +2714,7 @@
     <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
@@ -2723,7 +2731,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
@@ -2742,16 +2750,16 @@
       <c r="G4">
         <v>827.3</v>
       </c>
-      <c r="I4">
-        <f>(B4-G4)/G4</f>
+      <c r="I4" s="4">
+        <f t="shared" ref="I4:I36" si="0">(B4-G4)/G4</f>
         <v>5.011751749331838E-2</v>
       </c>
-      <c r="K4">
-        <f>(E4-G4)/G4</f>
+      <c r="K4" s="4">
+        <f t="shared" ref="K4:K36" si="1">(E4-G4)/G4</f>
         <v>3.9780007252508263E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="2" t="s">
         <v>32</v>
       </c>
@@ -2770,16 +2778,16 @@
       <c r="G5">
         <v>827.3</v>
       </c>
-      <c r="I5">
-        <f>(B5-G5)/G5</f>
+      <c r="I5" s="4">
+        <f t="shared" si="0"/>
         <v>4.754260848543454E-2</v>
       </c>
-      <c r="K5">
-        <f>(E5-G5)/G5</f>
+      <c r="K5" s="4">
+        <f t="shared" si="1"/>
         <v>4.0710745799589103E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
@@ -2798,16 +2806,16 @@
       <c r="G6">
         <v>826.3</v>
       </c>
-      <c r="I6">
-        <f>(B6-G6)/G6</f>
+      <c r="I6" s="4">
+        <f t="shared" si="0"/>
         <v>4.8489652668522343E-2</v>
       </c>
-      <c r="K6">
-        <f>(E6-G6)/G6</f>
+      <c r="K6" s="4">
+        <f t="shared" si="1"/>
         <v>4.6012344184920846E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
@@ -2826,16 +2834,16 @@
       <c r="G7">
         <v>822.9</v>
       </c>
-      <c r="I7">
-        <f>(B7-G7)/G7</f>
+      <c r="I7" s="4">
+        <f t="shared" si="0"/>
         <v>4.7674079475027338E-2</v>
       </c>
-      <c r="K7">
-        <f>(E7-G7)/G7</f>
+      <c r="K7" s="4">
+        <f t="shared" si="1"/>
         <v>4.6396889050917565E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="2" t="s">
         <v>29</v>
       </c>
@@ -2854,16 +2862,16 @@
       <c r="G8">
         <v>827.3</v>
       </c>
-      <c r="I8">
-        <f>(B8-G8)/G8</f>
+      <c r="I8" s="4">
+        <f t="shared" si="0"/>
         <v>4.6150126918893003E-2</v>
       </c>
-      <c r="K8">
-        <f>(E8-G8)/G8</f>
+      <c r="K8" s="4">
+        <f t="shared" si="1"/>
         <v>2.9578145775414032E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
@@ -2882,16 +2890,16 @@
       <c r="G9">
         <v>827.3</v>
       </c>
-      <c r="I9">
-        <f>(B9-G9)/G9</f>
+      <c r="I9" s="4">
+        <f t="shared" si="0"/>
         <v>4.7389097062734108E-2</v>
       </c>
-      <c r="K9">
-        <f>(E9-G9)/G9</f>
+      <c r="K9" s="4">
+        <f t="shared" si="1"/>
         <v>4.6778677626012385E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
@@ -2910,16 +2918,16 @@
       <c r="G10">
         <v>827.3</v>
       </c>
-      <c r="I10">
-        <f>(B10-G10)/G10</f>
+      <c r="I10" s="4">
+        <f t="shared" si="0"/>
         <v>5.7125589266288052E-2</v>
       </c>
-      <c r="K10">
-        <f>(E10-G10)/G10</f>
+      <c r="K10" s="4">
+        <f t="shared" si="1"/>
         <v>3.9780007252508263E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
@@ -2938,16 +2946,16 @@
       <c r="G11">
         <v>827.3</v>
       </c>
-      <c r="I11">
-        <f>(B11-G11)/G11</f>
+      <c r="I11" s="4">
+        <f t="shared" si="0"/>
         <v>5.2556509126072792E-2</v>
       </c>
-      <c r="K11">
-        <f>(E11-G11)/G11</f>
+      <c r="K11" s="4">
+        <f t="shared" si="1"/>
         <v>4.1581046778677737E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
@@ -2966,16 +2974,16 @@
       <c r="G12">
         <v>827.3</v>
       </c>
-      <c r="I12">
-        <f>(B12-G12)/G12</f>
+      <c r="I12" s="4">
+        <f t="shared" si="0"/>
         <v>6.3716910431524193E-2</v>
       </c>
-      <c r="K12">
-        <f>(E12-G12)/G12</f>
+      <c r="K12" s="4">
+        <f t="shared" si="1"/>
         <v>4.8724767315363307E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -2994,16 +3002,16 @@
       <c r="G13">
         <v>589.1</v>
       </c>
-      <c r="I13">
-        <f>(B13-G13)/G13</f>
+      <c r="I13" s="4">
+        <f t="shared" si="0"/>
         <v>0.13649804786963174</v>
       </c>
-      <c r="K13">
-        <f>(E13-G13)/G13</f>
+      <c r="K13" s="4">
+        <f t="shared" si="1"/>
         <v>0.12193176031234074</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
@@ -3022,16 +3030,16 @@
       <c r="G14">
         <v>589.1</v>
       </c>
-      <c r="I14">
-        <f>(B14-G14)/G14</f>
+      <c r="I14" s="4">
+        <f t="shared" si="0"/>
         <v>0.14026481072822949</v>
       </c>
-      <c r="K14">
-        <f>(E14-G14)/G14</f>
+      <c r="K14" s="4">
+        <f t="shared" si="1"/>
         <v>0.12361228993379721</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -3050,16 +3058,16 @@
       <c r="G15">
         <v>588.70000000000005</v>
       </c>
-      <c r="I15">
-        <f>(B15-G15)/G15</f>
+      <c r="I15" s="4">
+        <f t="shared" si="0"/>
         <v>0.11359266179717996</v>
       </c>
-      <c r="K15">
-        <f>(E15-G15)/G15</f>
+      <c r="K15" s="4">
+        <f t="shared" si="1"/>
         <v>9.8131476133854215E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
@@ -3078,16 +3086,16 @@
       <c r="G16">
         <v>588.1</v>
       </c>
-      <c r="I16">
-        <f>(B16-G16)/G16</f>
+      <c r="I16" s="4">
+        <f t="shared" si="0"/>
         <v>0.12090970923312357</v>
       </c>
-      <c r="K16">
-        <f>(E16-G16)/G16</f>
+      <c r="K16" s="4">
+        <f t="shared" si="1"/>
         <v>0.11054242475769425</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
@@ -3106,16 +3114,16 @@
       <c r="G17">
         <v>586.4</v>
       </c>
-      <c r="I17">
-        <f>(B17-G17)/G17</f>
+      <c r="I17" s="4">
+        <f t="shared" si="0"/>
         <v>0.12276773533424301</v>
       </c>
-      <c r="K17">
-        <f>(E17-G17)/G17</f>
+      <c r="K17" s="4">
+        <f t="shared" si="1"/>
         <v>9.3912005457026007E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
@@ -3134,16 +3142,16 @@
       <c r="G18">
         <v>586</v>
       </c>
-      <c r="I18">
-        <f>(B18-G18)/G18</f>
+      <c r="I18" s="4">
+        <f t="shared" si="0"/>
         <v>0.13199658703071676</v>
       </c>
-      <c r="K18">
-        <f>(E18-G18)/G18</f>
+      <c r="K18" s="4">
+        <f t="shared" si="1"/>
         <v>0.12102389078498287</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -3162,16 +3170,16 @@
       <c r="G19">
         <v>585.79999999999995</v>
       </c>
-      <c r="I19">
-        <f>(B19-G19)/G19</f>
+      <c r="I19" s="4">
+        <f t="shared" si="0"/>
         <v>0.1369614202799592</v>
       </c>
-      <c r="K19">
-        <f>(E19-G19)/G19</f>
+      <c r="K19" s="4">
+        <f t="shared" si="1"/>
         <v>0.1077842266985321</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
@@ -3190,16 +3198,16 @@
       <c r="G20">
         <v>585.79999999999995</v>
       </c>
-      <c r="I20">
-        <f>(B20-G20)/G20</f>
+      <c r="I20" s="4">
+        <f t="shared" si="0"/>
         <v>0.11436155684533961</v>
       </c>
-      <c r="K20">
-        <f>(E20-G20)/G20</f>
+      <c r="K20" s="4">
+        <f t="shared" si="1"/>
         <v>8.7726186411744803E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="2" t="s">
         <v>16</v>
       </c>
@@ -3218,16 +3226,16 @@
       <c r="G21">
         <v>1619.8</v>
       </c>
-      <c r="I21">
-        <f>(B21-G21)/G21</f>
+      <c r="I21" s="4">
+        <f t="shared" si="0"/>
         <v>3.6306334115322858E-2</v>
       </c>
-      <c r="K21">
-        <f>(E21-G21)/G21</f>
+      <c r="K21" s="4">
+        <f t="shared" si="1"/>
         <v>2.1447092233609095E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="2" t="s">
         <v>15</v>
       </c>
@@ -3246,16 +3254,16 @@
       <c r="G22">
         <v>1457.4</v>
       </c>
-      <c r="I22">
-        <f>(B22-G22)/G22</f>
+      <c r="I22" s="4">
+        <f t="shared" si="0"/>
         <v>3.5405516673528134E-2</v>
       </c>
-      <c r="K22">
-        <f>(E22-G22)/G22</f>
+      <c r="K22" s="4">
+        <f t="shared" si="1"/>
         <v>2.8283244133388088E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="2" t="s">
         <v>14</v>
       </c>
@@ -3274,16 +3282,16 @@
       <c r="G23">
         <v>1258</v>
       </c>
-      <c r="I23">
-        <f>(B23-G23)/G23</f>
+      <c r="I23" s="4">
+        <f t="shared" si="0"/>
         <v>7.7107313195548477E-2</v>
       </c>
-      <c r="K23">
-        <f>(E23-G23)/G23</f>
+      <c r="K23" s="4">
+        <f t="shared" si="1"/>
         <v>5.8537360890302148E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="2" t="s">
         <v>13</v>
       </c>
@@ -3302,16 +3310,16 @@
       <c r="G24">
         <v>1132.3</v>
       </c>
-      <c r="I24">
-        <f>(B24-G24)/G24</f>
+      <c r="I24" s="4">
+        <f t="shared" si="0"/>
         <v>4.5782919720921945E-2</v>
       </c>
-      <c r="K24">
-        <f>(E24-G24)/G24</f>
+      <c r="K24" s="4">
+        <f t="shared" si="1"/>
         <v>2.8349377373487715E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
@@ -3330,16 +3338,16 @@
       <c r="G25">
         <v>1513.7</v>
       </c>
-      <c r="I25">
-        <f>(B25-G25)/G25</f>
+      <c r="I25" s="4">
+        <f t="shared" si="0"/>
         <v>4.4508158816145914E-2</v>
       </c>
-      <c r="K25">
-        <f>(E25-G25)/G25</f>
+      <c r="K25" s="4">
+        <f t="shared" si="1"/>
         <v>3.6493360639492642E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="2" t="s">
         <v>11</v>
       </c>
@@ -3358,16 +3366,16 @@
       <c r="G26">
         <v>1372.7</v>
       </c>
-      <c r="I26">
-        <f>(B26-G26)/G26</f>
+      <c r="I26" s="4">
+        <f t="shared" si="0"/>
         <v>3.3072047789029023E-2</v>
       </c>
-      <c r="K26">
-        <f>(E26-G26)/G26</f>
+      <c r="K26" s="4">
+        <f t="shared" si="1"/>
         <v>1.7935455671304647E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27" s="2" t="s">
         <v>10</v>
       </c>
@@ -3386,16 +3394,16 @@
       <c r="G27">
         <v>1207.8</v>
       </c>
-      <c r="I27">
-        <f>(B27-G27)/G27</f>
+      <c r="I27" s="4">
+        <f t="shared" si="0"/>
         <v>6.6288292763702503E-2</v>
       </c>
-      <c r="K27">
-        <f>(E27-G27)/G27</f>
+      <c r="K27" s="4">
+        <f t="shared" si="1"/>
         <v>3.8565987746315741E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" s="2" t="s">
         <v>9</v>
       </c>
@@ -3414,16 +3422,16 @@
       <c r="G28">
         <v>1114.2</v>
       </c>
-      <c r="I28">
-        <f>(B28-G28)/G28</f>
+      <c r="I28" s="4">
+        <f t="shared" si="0"/>
         <v>4.6107521091365837E-2</v>
       </c>
-      <c r="K28">
-        <f>(E28-G28)/G28</f>
+      <c r="K28" s="4">
+        <f t="shared" si="1"/>
         <v>3.8305510680308796E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -3442,16 +3450,16 @@
       <c r="G29">
         <v>1261.8</v>
       </c>
-      <c r="I29">
-        <f>(B29-G29)/G29</f>
+      <c r="I29" s="4">
+        <f t="shared" si="0"/>
         <v>2.1692027262640568E-2</v>
       </c>
-      <c r="K29">
-        <f>(E29-G29)/G29</f>
+      <c r="K29" s="4">
+        <f t="shared" si="1"/>
         <v>1.1602472658107545E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30" s="2" t="s">
         <v>7</v>
       </c>
@@ -3470,16 +3478,16 @@
       <c r="G30">
         <v>1092.3</v>
       </c>
-      <c r="I30">
-        <f>(B30-G30)/G30</f>
+      <c r="I30" s="4">
+        <f t="shared" si="0"/>
         <v>3.5977295614757855E-2</v>
       </c>
-      <c r="K30">
-        <f>(E30-G30)/G30</f>
+      <c r="K30" s="4">
+        <f t="shared" si="1"/>
         <v>2.0186761878604739E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31" s="2" t="s">
         <v>6</v>
       </c>
@@ -3498,16 +3506,16 @@
       <c r="G31">
         <v>923.7</v>
       </c>
-      <c r="I31">
-        <f>(B31-G31)/G31</f>
+      <c r="I31" s="4">
+        <f t="shared" si="0"/>
         <v>3.3646205477968857E-2</v>
       </c>
-      <c r="K31">
-        <f>(E31-G31)/G31</f>
+      <c r="K31" s="4">
+        <f t="shared" si="1"/>
         <v>1.5264696329977167E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32" s="2" t="s">
         <v>5</v>
       </c>
@@ -3526,16 +3534,16 @@
       <c r="G32">
         <v>783.5</v>
       </c>
-      <c r="I32">
-        <f>(B32-G32)/G32</f>
+      <c r="I32" s="4">
+        <f t="shared" si="0"/>
         <v>2.9783024888321682E-2</v>
       </c>
-      <c r="K32">
-        <f>(E32-G32)/G32</f>
+      <c r="K32" s="4">
+        <f t="shared" si="1"/>
         <v>2.1786853860880726E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11">
       <c r="A33" s="2" t="s">
         <v>4</v>
       </c>
@@ -3554,16 +3562,16 @@
       <c r="G33">
         <v>1154</v>
       </c>
-      <c r="I33">
-        <f>(B33-G33)/G33</f>
+      <c r="I33" s="4">
+        <f t="shared" si="0"/>
         <v>2.2990467937608471E-2</v>
       </c>
-      <c r="K33">
-        <f>(E33-G33)/G33</f>
+      <c r="K33" s="4">
+        <f t="shared" si="1"/>
         <v>1.8284228769497323E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11">
       <c r="A34" s="2" t="s">
         <v>3</v>
       </c>
@@ -3582,16 +3590,16 @@
       <c r="G34">
         <v>1051.0999999999999</v>
       </c>
-      <c r="I34">
-        <f>(B34-G34)/G34</f>
+      <c r="I34" s="4">
+        <f t="shared" si="0"/>
         <v>3.1798116259157079E-2</v>
       </c>
-      <c r="K34">
-        <f>(E34-G34)/G34</f>
+      <c r="K34" s="4">
+        <f t="shared" si="1"/>
         <v>6.4028160974217664E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11">
       <c r="A35" s="2" t="s">
         <v>2</v>
       </c>
@@ -3610,16 +3618,16 @@
       <c r="G35">
         <v>962.9</v>
       </c>
-      <c r="I35">
-        <f>(B35-G35)/G35</f>
+      <c r="I35" s="4">
+        <f t="shared" si="0"/>
         <v>4.2312805068023734E-2</v>
       </c>
-      <c r="K35">
-        <f>(E35-G35)/G35</f>
+      <c r="K35" s="4">
+        <f t="shared" si="1"/>
         <v>2.944230968947972E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11">
       <c r="A36" s="2" t="s">
         <v>1</v>
       </c>
@@ -3638,16 +3646,16 @@
       <c r="G36">
         <v>776.1</v>
       </c>
-      <c r="I36">
-        <f>(B36-G36)/G36</f>
+      <c r="I36" s="4">
+        <f t="shared" si="0"/>
         <v>2.8926684705579089E-2</v>
       </c>
-      <c r="K36">
-        <f>(E36-G36)/G36</f>
+      <c r="K36" s="4">
+        <f t="shared" si="1"/>
         <v>8.5040587553150658E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11">
       <c r="A37" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>